<commit_message>
testing: downloader and rename cta button
</commit_message>
<xml_diff>
--- a/backend/usage_2025_06.xlsx
+++ b/backend/usage_2025_06.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Laporan Penggunaan Inventaris</t>
   </si>
@@ -28,28 +28,22 @@
     <t>Jumlah Digunakan</t>
   </si>
   <si>
+    <t>Kampus dan Ruangan</t>
+  </si>
+  <si>
     <t>Tanggal Pemasangan</t>
   </si>
   <si>
-    <t>Kabel LAB CAT26</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>D112</t>
   </si>
   <si>
     <t>2025-06-05</t>
-  </si>
-  <si>
-    <t>Lampu LED</t>
-  </si>
-  <si>
-    <t>USB TYPE A</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>USB TYPE C</t>
   </si>
 </sst>
 </file>
@@ -379,60 +373,19 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>